<commit_message>
Demo 2 plan de test logiciel
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Demo2/Plans de test logiciel demo 2.xlsx
+++ b/Documentation/Tests/Demo2/Plans de test logiciel demo 2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="110">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -365,6 +365,13 @@
   </si>
   <si>
     <t>moins 3,009dB à 7000Hz</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Déjà testé dans le
+ plan d'intégration</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1330,59 +1337,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1413,59 +1381,266 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1473,9 +1648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1509,161 +1681,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1968,7 +2008,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1996,16 +2036,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="66" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+      <c r="F2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="56"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2014,16 +2054,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
-      <c r="F3" s="70" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="F3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="71"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2032,22 +2072,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="74" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="43" t="s">
+      <c r="F5" s="68"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="45"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2062,181 +2102,181 @@
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="58"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="75"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="61"/>
+      <c r="O6" s="48"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="60"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="65"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="62"/>
+      <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="60"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="65"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="62"/>
+      <c r="O8" s="49"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="60"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="62"/>
+      <c r="O9" s="49"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="65"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="62"/>
+      <c r="O10" s="49"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="60"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="62"/>
+      <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="60"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="65"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="62"/>
+      <c r="O12" s="49"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="60"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="62"/>
+      <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="60"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="65"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="62"/>
+      <c r="O14" s="49"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="54"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="63"/>
+      <c r="O15" s="50"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2251,6 +2291,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="O6:O15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -2267,30 +2331,6 @@
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2301,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,16 +2359,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="66" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
+      <c r="F2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="56"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2337,16 +2377,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
-      <c r="F3" s="70" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="F3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="71"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2355,22 +2395,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="74" t="s">
+      <c r="C5" s="68"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="43" t="s">
+      <c r="F5" s="68"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="45"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="72"/>
       <c r="L5" s="13" t="s">
         <v>7</v>
       </c>
@@ -2385,496 +2425,526 @@
       <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="73"/>
-      <c r="O6" s="61"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="145"/>
+      <c r="L6" s="145"/>
+      <c r="M6" s="62"/>
+      <c r="O6" s="48"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="92" t="s">
+      <c r="C7" s="68"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="149"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="72"/>
       <c r="L7" s="36"/>
       <c r="M7" s="36"/>
-      <c r="O7" s="62"/>
+      <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="81" t="s">
+      <c r="C8" s="83"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="82"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="81" t="s">
+      <c r="F8" s="83"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="84"/>
       <c r="L8" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M8" s="34"/>
-      <c r="O8" s="62"/>
+      <c r="O8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="75" t="s">
+      <c r="C9" s="89"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="76"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="75" t="s">
+      <c r="F9" s="89"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="77"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="90"/>
       <c r="L9" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M9" s="34"/>
-      <c r="O9" s="62"/>
+      <c r="O9" s="49"/>
     </row>
     <row r="10" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="75" t="s">
+      <c r="C10" s="89"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="76"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="75" t="s">
+      <c r="F10" s="89"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="77"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="90"/>
       <c r="L10" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M10" s="34"/>
-      <c r="O10" s="62"/>
+      <c r="O10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="75" t="s">
+      <c r="C11" s="89"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="75" t="s">
+      <c r="F11" s="89"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="77"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="90"/>
       <c r="L11" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M11" s="34"/>
-      <c r="O11" s="62"/>
+      <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="78" t="s">
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="79"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="75" t="s">
+      <c r="F12" s="159"/>
+      <c r="G12" s="160"/>
+      <c r="H12" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="77"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="90"/>
       <c r="L12" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M12" s="41"/>
-      <c r="O12" s="62"/>
+      <c r="O12" s="49"/>
     </row>
     <row r="13" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="42">
         <v>1.2</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="95" t="s">
+      <c r="C13" s="68"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="45"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="72"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
-      <c r="O13" s="62"/>
+      <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="150"/>
-      <c r="D14" s="151"/>
-      <c r="E14" s="81" t="s">
+      <c r="C14" s="81"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="150"/>
-      <c r="G14" s="151"/>
-      <c r="H14" s="81" t="s">
+      <c r="F14" s="81"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="I14" s="82"/>
-      <c r="J14" s="82"/>
-      <c r="K14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="84"/>
       <c r="L14" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M14" s="34"/>
-      <c r="O14" s="62"/>
+      <c r="O14" s="49"/>
     </row>
     <row r="15" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="75" t="s">
+      <c r="C15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="127"/>
-      <c r="G15" s="128"/>
-      <c r="H15" s="81" t="s">
+      <c r="F15" s="86"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="82"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="84"/>
       <c r="L15" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M15" s="40"/>
-      <c r="O15" s="62"/>
+      <c r="O15" s="49"/>
     </row>
     <row r="16" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="127"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="75" t="s">
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="127"/>
-      <c r="G16" s="128"/>
-      <c r="H16" s="81" t="s">
+      <c r="F16" s="86"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="83"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="84"/>
       <c r="L16" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M16" s="40"/>
-      <c r="O16" s="62"/>
+      <c r="O16" s="49"/>
     </row>
     <row r="17" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="127"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="75" t="s">
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="127"/>
-      <c r="G17" s="128"/>
-      <c r="H17" s="75" t="s">
+      <c r="F17" s="86"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="77"/>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="90"/>
       <c r="L17" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M17" s="40"/>
-      <c r="O17" s="62"/>
+      <c r="O17" s="49"/>
     </row>
     <row r="18" spans="1:15" s="35" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="127"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="75" t="s">
+      <c r="C18" s="86"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="127"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="75" t="s">
+      <c r="F18" s="86"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="77"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="90"/>
       <c r="L18" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M18" s="40"/>
-      <c r="O18" s="62"/>
+      <c r="O18" s="49"/>
     </row>
     <row r="19" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>1.3</v>
       </c>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="87" t="s">
+      <c r="C19" s="64"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="88"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="O19" s="62"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="164" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="M19" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="49"/>
     </row>
     <row r="20" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>1.4</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="87" t="s">
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="88"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="O20" s="62"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="161" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="162"/>
+      <c r="L20" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="M20" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="49"/>
     </row>
     <row r="21" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>1.5</v>
       </c>
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="90" t="s">
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="146" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="O21" s="62"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="161" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="162"/>
+      <c r="L21" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="M21" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O21" s="49"/>
     </row>
     <row r="22" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>1.6</v>
       </c>
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="87" t="s">
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="88"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="O22" s="62"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="161" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="162"/>
+      <c r="L22" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O22" s="49"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <v>1.7</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="143" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="107" t="s">
+      <c r="C23" s="140"/>
+      <c r="D23" s="141"/>
+      <c r="E23" s="110" t="s">
         <v>27</v>
       </c>
       <c r="F23" s="108"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="O23" s="62"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="163" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="108"/>
+      <c r="J23" s="108"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="49"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20">
         <v>2</v>
       </c>
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="156" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="102"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="103"/>
-      <c r="O24" s="62"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="157"/>
+      <c r="M24" s="158"/>
+      <c r="O24" s="49"/>
     </row>
     <row r="25" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>2.1</v>
       </c>
-      <c r="B25" s="96" t="s">
+      <c r="B25" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="97"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="99" t="s">
+      <c r="C25" s="152"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="68"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="155"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="56"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
-      <c r="O25" s="63"/>
+      <c r="O25" s="50"/>
     </row>
     <row r="26" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B26" s="115" t="s">
+      <c r="B26" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="105"/>
-      <c r="D26" s="106"/>
-      <c r="E26" s="104" t="s">
+      <c r="C26" s="140"/>
+      <c r="D26" s="141"/>
+      <c r="E26" s="143" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="106"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="141"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="141"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
       <c r="O26" s="2"/>
@@ -2883,434 +2953,536 @@
       <c r="A27" s="20">
         <v>3</v>
       </c>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="85"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="85"/>
-      <c r="M27" s="73"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="145"/>
+      <c r="L27" s="145"/>
+      <c r="M27" s="62"/>
     </row>
     <row r="28" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>3.1</v>
       </c>
-      <c r="B28" s="111" t="s">
+      <c r="B28" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="112" t="s">
+      <c r="C28" s="74"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="113"/>
-      <c r="G28" s="114"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="96"/>
+      <c r="H28" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="166"/>
+      <c r="L28" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M28" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>3.2</v>
       </c>
-      <c r="B29" s="86" t="s">
+      <c r="B29" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="87" t="s">
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="88"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="166"/>
+      <c r="L29" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M29" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="30" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>3.3</v>
       </c>
-      <c r="B30" s="86" t="s">
+      <c r="B30" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="87" t="s">
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="166"/>
+      <c r="L30" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M30" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="31" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <v>3.4</v>
       </c>
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="125"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="75" t="s">
+      <c r="C31" s="133"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="127"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="129"/>
-      <c r="I31" s="130"/>
-      <c r="J31" s="130"/>
-      <c r="K31" s="131"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="166"/>
+      <c r="L31" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M31" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="32" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
         <v>3.5</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="119"/>
-      <c r="D32" s="120"/>
-      <c r="E32" s="78" t="s">
+      <c r="C32" s="115"/>
+      <c r="D32" s="116"/>
+      <c r="E32" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="119"/>
-      <c r="G32" s="120"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="122"/>
-      <c r="J32" s="122"/>
-      <c r="K32" s="123"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="116"/>
+      <c r="H32" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="95"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="166"/>
+      <c r="L32" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M32" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <v>4</v>
       </c>
-      <c r="B33" s="116" t="s">
+      <c r="B33" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="117"/>
-      <c r="I33" s="117"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="117"/>
-      <c r="L33" s="117"/>
-      <c r="M33" s="118"/>
+      <c r="C33" s="136"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="136"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="136"/>
+      <c r="J33" s="136"/>
+      <c r="K33" s="136"/>
+      <c r="L33" s="136"/>
+      <c r="M33" s="137"/>
     </row>
     <row r="34" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="112" t="s">
+      <c r="C34" s="74"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="113"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="95"/>
+      <c r="J34" s="95"/>
+      <c r="K34" s="166"/>
+      <c r="L34" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M34" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>4.2</v>
       </c>
-      <c r="B35" s="86" t="s">
+      <c r="B35" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="112" t="s">
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="113"/>
-      <c r="G35" s="114"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I35" s="95"/>
+      <c r="J35" s="95"/>
+      <c r="K35" s="166"/>
+      <c r="L35" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M35" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>4.3</v>
       </c>
-      <c r="B36" s="86" t="s">
+      <c r="B36" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="87" t="s">
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="95"/>
+      <c r="J36" s="95"/>
+      <c r="K36" s="166"/>
+      <c r="L36" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M36" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B37" s="86" t="s">
+      <c r="B37" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="87" t="s">
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="88"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
+      <c r="F37" s="92"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="95"/>
+      <c r="J37" s="95"/>
+      <c r="K37" s="166"/>
+      <c r="L37" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M37" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="38" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <v>4.5</v>
       </c>
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="125"/>
-      <c r="D38" s="126"/>
-      <c r="E38" s="112" t="s">
+      <c r="C38" s="133"/>
+      <c r="D38" s="134"/>
+      <c r="E38" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="113"/>
-      <c r="G38" s="114"/>
-      <c r="H38" s="129"/>
-      <c r="I38" s="130"/>
-      <c r="J38" s="130"/>
-      <c r="K38" s="131"/>
-      <c r="L38" s="16"/>
-      <c r="M38" s="16"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="95"/>
+      <c r="J38" s="95"/>
+      <c r="K38" s="166"/>
+      <c r="L38" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M38" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="39" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B39" s="124" t="s">
+      <c r="B39" s="132" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="125"/>
-      <c r="D39" s="126"/>
-      <c r="E39" s="87" t="s">
+      <c r="C39" s="133"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="129"/>
-      <c r="I39" s="130"/>
-      <c r="J39" s="130"/>
-      <c r="K39" s="131"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
+      <c r="K39" s="166"/>
+      <c r="L39" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M39" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21">
         <v>4.7</v>
       </c>
-      <c r="B40" s="86" t="s">
+      <c r="B40" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="87" t="s">
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="88"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="129"/>
-      <c r="I40" s="130"/>
-      <c r="J40" s="130"/>
-      <c r="K40" s="131"/>
-      <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" s="95"/>
+      <c r="J40" s="95"/>
+      <c r="K40" s="166"/>
+      <c r="L40" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M40" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>4.8</v>
       </c>
-      <c r="B41" s="86" t="s">
+      <c r="B41" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="87" t="s">
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="88"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="129"/>
-      <c r="I41" s="130"/>
-      <c r="J41" s="130"/>
-      <c r="K41" s="131"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="95"/>
+      <c r="J41" s="95"/>
+      <c r="K41" s="166"/>
+      <c r="L41" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="125"/>
-      <c r="D42" s="126"/>
-      <c r="E42" s="112" t="s">
+      <c r="C42" s="133"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="113"/>
-      <c r="G42" s="114"/>
-      <c r="H42" s="129"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="130"/>
-      <c r="K42" s="131"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
+      <c r="F42" s="95"/>
+      <c r="G42" s="96"/>
+      <c r="H42" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" s="95"/>
+      <c r="J42" s="95"/>
+      <c r="K42" s="166"/>
+      <c r="L42" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M42" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="43" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B43" s="124" t="s">
+      <c r="B43" s="132" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="125"/>
-      <c r="D43" s="126"/>
-      <c r="E43" s="87" t="s">
+      <c r="C43" s="133"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="88"/>
-      <c r="G43" s="89"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="130"/>
-      <c r="J43" s="130"/>
-      <c r="K43" s="131"/>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
+      <c r="F43" s="92"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I43" s="95"/>
+      <c r="J43" s="95"/>
+      <c r="K43" s="166"/>
+      <c r="L43" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M43" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B44" s="86" t="s">
+      <c r="B44" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="50"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="87" t="s">
+      <c r="C44" s="64"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="88"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="129"/>
-      <c r="I44" s="130"/>
-      <c r="J44" s="130"/>
-      <c r="K44" s="131"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="95"/>
+      <c r="J44" s="95"/>
+      <c r="K44" s="166"/>
+      <c r="L44" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M44" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>4.12</v>
       </c>
-      <c r="B45" s="145" t="s">
+      <c r="B45" s="107" t="s">
         <v>56</v>
       </c>
       <c r="C45" s="108"/>
-      <c r="D45" s="146"/>
-      <c r="E45" s="107" t="s">
+      <c r="D45" s="109"/>
+      <c r="E45" s="110" t="s">
         <v>46</v>
       </c>
       <c r="F45" s="108"/>
-      <c r="G45" s="146"/>
-      <c r="H45" s="121"/>
-      <c r="I45" s="122"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="123"/>
-      <c r="L45" s="16"/>
-      <c r="M45" s="16"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="165" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="95"/>
+      <c r="J45" s="95"/>
+      <c r="K45" s="166"/>
+      <c r="L45" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="M45" s="47" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="25">
         <v>5</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="139"/>
-      <c r="D46" s="139"/>
-      <c r="E46" s="139"/>
-      <c r="F46" s="139"/>
-      <c r="G46" s="139"/>
-      <c r="H46" s="139"/>
-      <c r="I46" s="139"/>
-      <c r="J46" s="139"/>
-      <c r="K46" s="139"/>
-      <c r="L46" s="139"/>
-      <c r="M46" s="140"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="118"/>
+      <c r="I46" s="118"/>
+      <c r="J46" s="118"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="118"/>
+      <c r="M46" s="119"/>
     </row>
     <row r="47" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B47" s="152" t="s">
+      <c r="B47" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="153"/>
-      <c r="D47" s="154"/>
-      <c r="E47" s="152" t="s">
+      <c r="C47" s="121"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="120" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="153"/>
-      <c r="G47" s="154"/>
-      <c r="H47" s="155"/>
-      <c r="I47" s="155"/>
-      <c r="J47" s="155"/>
-      <c r="K47" s="155"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="122"/>
+      <c r="H47" s="123"/>
+      <c r="I47" s="123"/>
+      <c r="J47" s="123"/>
+      <c r="K47" s="123"/>
       <c r="L47" s="30"/>
       <c r="M47" s="32" t="s">
         <v>60</v>
@@ -3320,20 +3492,20 @@
       <c r="A48" s="28">
         <v>5.2</v>
       </c>
-      <c r="B48" s="142" t="s">
+      <c r="B48" s="104" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="143"/>
-      <c r="D48" s="144"/>
-      <c r="E48" s="142" t="s">
+      <c r="C48" s="105"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="143"/>
-      <c r="G48" s="144"/>
-      <c r="H48" s="141"/>
-      <c r="I48" s="141"/>
-      <c r="J48" s="141"/>
-      <c r="K48" s="141"/>
+      <c r="F48" s="105"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="124"/>
+      <c r="I48" s="124"/>
+      <c r="J48" s="124"/>
+      <c r="K48" s="124"/>
       <c r="L48" s="19"/>
       <c r="M48" s="16"/>
     </row>
@@ -3341,20 +3513,20 @@
       <c r="A49" s="28">
         <v>5.3</v>
       </c>
-      <c r="B49" s="142" t="s">
+      <c r="B49" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="143"/>
-      <c r="D49" s="144"/>
-      <c r="E49" s="142" t="s">
+      <c r="C49" s="105"/>
+      <c r="D49" s="106"/>
+      <c r="E49" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="143"/>
-      <c r="G49" s="144"/>
-      <c r="H49" s="141"/>
-      <c r="I49" s="141"/>
-      <c r="J49" s="141"/>
-      <c r="K49" s="141"/>
+      <c r="F49" s="105"/>
+      <c r="G49" s="106"/>
+      <c r="H49" s="124"/>
+      <c r="I49" s="124"/>
+      <c r="J49" s="124"/>
+      <c r="K49" s="124"/>
       <c r="L49" s="19"/>
       <c r="M49" s="16"/>
     </row>
@@ -3362,20 +3534,20 @@
       <c r="A50" s="29">
         <v>5.4</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="119"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="78" t="s">
+      <c r="C50" s="115"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="F50" s="119"/>
-      <c r="G50" s="120"/>
-      <c r="H50" s="121"/>
-      <c r="I50" s="122"/>
-      <c r="J50" s="122"/>
-      <c r="K50" s="123"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
+      <c r="K50" s="113"/>
       <c r="L50" s="23"/>
       <c r="M50" s="16"/>
     </row>
@@ -3383,39 +3555,39 @@
       <c r="A51" s="25">
         <v>6</v>
       </c>
-      <c r="B51" s="92" t="s">
+      <c r="B51" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="139"/>
-      <c r="D51" s="139"/>
-      <c r="E51" s="139"/>
-      <c r="F51" s="139"/>
-      <c r="G51" s="139"/>
-      <c r="H51" s="139"/>
-      <c r="I51" s="139"/>
-      <c r="J51" s="139"/>
-      <c r="K51" s="139"/>
-      <c r="L51" s="139"/>
-      <c r="M51" s="140"/>
+      <c r="C51" s="118"/>
+      <c r="D51" s="118"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="118"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="118"/>
+      <c r="I51" s="118"/>
+      <c r="J51" s="118"/>
+      <c r="K51" s="118"/>
+      <c r="L51" s="118"/>
+      <c r="M51" s="119"/>
     </row>
     <row r="52" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
         <v>6.1</v>
       </c>
-      <c r="B52" s="81" t="s">
+      <c r="B52" s="80" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="150"/>
-      <c r="D52" s="151"/>
-      <c r="E52" s="81" t="s">
+      <c r="C52" s="81"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="F52" s="150"/>
-      <c r="G52" s="151"/>
-      <c r="H52" s="147"/>
-      <c r="I52" s="148"/>
-      <c r="J52" s="148"/>
-      <c r="K52" s="149"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="101"/>
+      <c r="I52" s="102"/>
+      <c r="J52" s="102"/>
+      <c r="K52" s="103"/>
       <c r="L52" s="30"/>
       <c r="M52" s="33"/>
     </row>
@@ -3423,20 +3595,20 @@
       <c r="A53" s="28">
         <v>6.2</v>
       </c>
-      <c r="B53" s="75" t="s">
+      <c r="B53" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="127"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="75" t="s">
+      <c r="C53" s="86"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="F53" s="127"/>
-      <c r="G53" s="128"/>
-      <c r="H53" s="129"/>
-      <c r="I53" s="130"/>
-      <c r="J53" s="130"/>
-      <c r="K53" s="131"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="87"/>
+      <c r="H53" s="98"/>
+      <c r="I53" s="99"/>
+      <c r="J53" s="99"/>
+      <c r="K53" s="100"/>
       <c r="L53" s="19"/>
       <c r="M53" s="16"/>
     </row>
@@ -3444,20 +3616,20 @@
       <c r="A54" s="28">
         <v>6.3</v>
       </c>
-      <c r="B54" s="81" t="s">
+      <c r="B54" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="150"/>
-      <c r="D54" s="151"/>
-      <c r="E54" s="81" t="s">
+      <c r="C54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="F54" s="150"/>
-      <c r="G54" s="151"/>
-      <c r="H54" s="129"/>
-      <c r="I54" s="130"/>
-      <c r="J54" s="130"/>
-      <c r="K54" s="131"/>
+      <c r="F54" s="81"/>
+      <c r="G54" s="82"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="99"/>
+      <c r="J54" s="99"/>
+      <c r="K54" s="100"/>
       <c r="L54" s="19"/>
       <c r="M54" s="16"/>
     </row>
@@ -3465,35 +3637,35 @@
       <c r="A55" s="28">
         <v>6.4</v>
       </c>
-      <c r="B55" s="142" t="s">
+      <c r="B55" s="104" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="143"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="142" t="s">
+      <c r="C55" s="105"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="143"/>
-      <c r="G55" s="144"/>
-      <c r="H55" s="141"/>
-      <c r="I55" s="141"/>
-      <c r="J55" s="141"/>
-      <c r="K55" s="141"/>
+      <c r="F55" s="105"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="124"/>
+      <c r="J55" s="124"/>
+      <c r="K55" s="124"/>
       <c r="L55" s="19"/>
       <c r="M55" s="16"/>
     </row>
     <row r="56" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
-      <c r="B56" s="132"/>
-      <c r="C56" s="133"/>
-      <c r="D56" s="134"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="133"/>
-      <c r="G56" s="134"/>
-      <c r="H56" s="136"/>
-      <c r="I56" s="137"/>
-      <c r="J56" s="137"/>
-      <c r="K56" s="138"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="126"/>
+      <c r="D56" s="127"/>
+      <c r="E56" s="128"/>
+      <c r="F56" s="126"/>
+      <c r="G56" s="127"/>
+      <c r="H56" s="129"/>
+      <c r="I56" s="130"/>
+      <c r="J56" s="130"/>
+      <c r="K56" s="131"/>
       <c r="L56" s="17"/>
       <c r="M56" s="6"/>
     </row>
@@ -3525,60 +3697,72 @@
     </row>
   </sheetData>
   <mergeCells count="151">
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="O6:O25"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="B27:M27"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="E56:G56"/>
     <mergeCell ref="H56:K56"/>
@@ -3603,6 +3787,51 @@
     <mergeCell ref="H55:K55"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="B33:M33"/>
@@ -3610,72 +3839,15 @@
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="O6:O25"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
encore tests logiciel demo2
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Demo2/Plans de test logiciel demo 2.xlsx
+++ b/Documentation/Tests/Demo2/Plans de test logiciel demo 2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -372,6 +372,9 @@
   <si>
     <t>Déjà testé dans le
  plan d'intégration</t>
+  </si>
+  <si>
+    <t>Tous les tests précédents ont été testés après quantifications des coefficients des filtres</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1352,6 +1355,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1381,234 +1438,264 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1617,93 +1704,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2008,7 +2008,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2036,16 +2036,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="F2" s="53" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="70"/>
+      <c r="F2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2054,16 +2054,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="78"/>
+      <c r="F3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2072,22 +2072,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="67" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="71" t="s">
+      <c r="F5" s="49"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="72"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="50"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2102,181 +2102,181 @@
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="63"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="48"/>
+      <c r="O6" s="66"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="65"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
       <c r="K7" s="65"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="49"/>
+      <c r="O7" s="67"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="65"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
       <c r="K8" s="65"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="49"/>
+      <c r="O8" s="67"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="65"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
       <c r="K9" s="65"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="49"/>
+      <c r="O9" s="67"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="65"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="65"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="49"/>
+      <c r="O10" s="67"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
       <c r="K11" s="65"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="49"/>
+      <c r="O11" s="67"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="65"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="65"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="49"/>
+      <c r="O12" s="67"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="65"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
       <c r="K13" s="65"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="49"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="65"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="65"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="49"/>
+      <c r="O14" s="67"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="50"/>
+      <c r="O15" s="68"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2291,6 +2291,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="O6:O15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
@@ -2307,30 +2331,6 @@
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O6:O15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2341,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,16 +2359,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="F2" s="53" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="70"/>
+      <c r="F2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2377,16 +2377,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="62"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="78"/>
+      <c r="F3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2395,22 +2395,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="67" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="71" t="s">
+      <c r="F5" s="49"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="72"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="50"/>
       <c r="L5" s="13" t="s">
         <v>7</v>
       </c>
@@ -2425,526 +2425,526 @@
       <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="144" t="s">
+      <c r="B6" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="145"/>
-      <c r="L6" s="145"/>
-      <c r="M6" s="62"/>
-      <c r="O6" s="48"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="78"/>
+      <c r="O6" s="66"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="147" t="s">
+      <c r="B7" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="117" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="148"/>
-      <c r="G7" s="149"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="72"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="36"/>
       <c r="M7" s="36"/>
-      <c r="O7" s="49"/>
+      <c r="O7" s="67"/>
     </row>
     <row r="8" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="80" t="s">
+      <c r="C8" s="87"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="80" t="s">
+      <c r="F8" s="87"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="84"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="88"/>
       <c r="L8" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M8" s="34"/>
-      <c r="O8" s="49"/>
+      <c r="O8" s="67"/>
     </row>
     <row r="9" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="89"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="85" t="s">
+      <c r="C9" s="81"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="89"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="85" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="90"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="82"/>
       <c r="L9" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M9" s="34"/>
-      <c r="O9" s="49"/>
+      <c r="O9" s="67"/>
     </row>
     <row r="10" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="85" t="s">
+      <c r="C10" s="81"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="85" t="s">
+      <c r="F10" s="81"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="90"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="82"/>
       <c r="L10" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M10" s="34"/>
-      <c r="O10" s="49"/>
+      <c r="O10" s="67"/>
     </row>
     <row r="11" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="80" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="89"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="85" t="s">
+      <c r="C11" s="81"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="89"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="85" t="s">
+      <c r="F11" s="81"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="90"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="82"/>
       <c r="L11" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M11" s="34"/>
-      <c r="O11" s="49"/>
+      <c r="O11" s="67"/>
     </row>
     <row r="12" spans="1:15" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="159"/>
-      <c r="D12" s="160"/>
-      <c r="E12" s="114" t="s">
+      <c r="C12" s="84"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="159"/>
-      <c r="G12" s="160"/>
-      <c r="H12" s="85" t="s">
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="90"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M12" s="41"/>
-      <c r="O12" s="49"/>
+      <c r="O12" s="67"/>
     </row>
     <row r="13" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="42">
         <v>1.2</v>
       </c>
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="150" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="68"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="72"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
-      <c r="O13" s="49"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="80" t="s">
+      <c r="C14" s="161"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="81"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="80" t="s">
+      <c r="F14" s="161"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="I14" s="83"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="84"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="88"/>
       <c r="L14" s="34" t="s">
         <v>87</v>
       </c>
       <c r="M14" s="34"/>
-      <c r="O14" s="49"/>
+      <c r="O14" s="67"/>
     </row>
     <row r="15" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="85" t="s">
+      <c r="C15" s="122"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="86"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="80" t="s">
+      <c r="F15" s="122"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="86" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="83"/>
-      <c r="J15" s="83"/>
-      <c r="K15" s="84"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="88"/>
       <c r="L15" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M15" s="40"/>
-      <c r="O15" s="49"/>
+      <c r="O15" s="67"/>
     </row>
     <row r="16" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="85" t="s">
+      <c r="C16" s="122"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="86"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="80" t="s">
+      <c r="F16" s="122"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="I16" s="83"/>
-      <c r="J16" s="83"/>
-      <c r="K16" s="84"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="88"/>
       <c r="L16" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M16" s="40"/>
-      <c r="O16" s="49"/>
+      <c r="O16" s="67"/>
     </row>
     <row r="17" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="85" t="s">
+      <c r="C17" s="122"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="86"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="85" t="s">
+      <c r="F17" s="122"/>
+      <c r="G17" s="123"/>
+      <c r="H17" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="89"/>
-      <c r="J17" s="89"/>
-      <c r="K17" s="90"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="82"/>
       <c r="L17" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M17" s="40"/>
-      <c r="O17" s="49"/>
+      <c r="O17" s="67"/>
     </row>
     <row r="18" spans="1:15" s="35" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="85" t="s">
+      <c r="C18" s="122"/>
+      <c r="D18" s="123"/>
+      <c r="E18" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="F18" s="86"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="85" t="s">
+      <c r="F18" s="122"/>
+      <c r="G18" s="123"/>
+      <c r="H18" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="89"/>
-      <c r="J18" s="89"/>
-      <c r="K18" s="90"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M18" s="40"/>
-      <c r="O18" s="49"/>
+      <c r="O18" s="67"/>
     </row>
     <row r="19" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>1.3</v>
       </c>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="64"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="65"/>
-      <c r="E19" s="91" t="s">
+      <c r="E19" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="164" t="s">
-        <v>108</v>
-      </c>
-      <c r="I19" s="89"/>
-      <c r="J19" s="89"/>
-      <c r="K19" s="90"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="82"/>
       <c r="L19" s="43" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="O19" s="49"/>
+        <v>110</v>
+      </c>
+      <c r="O19" s="67"/>
     </row>
     <row r="20" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>1.4</v>
       </c>
-      <c r="B20" s="88" t="s">
+      <c r="B20" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="65"/>
-      <c r="E20" s="91" t="s">
+      <c r="E20" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="92"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="161" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="162"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="96"/>
       <c r="L20" s="43" t="s">
         <v>108</v>
       </c>
       <c r="M20" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="O20" s="49"/>
+      <c r="O20" s="67"/>
     </row>
     <row r="21" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>1.5</v>
       </c>
-      <c r="B21" s="88" t="s">
+      <c r="B21" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="64"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="65"/>
-      <c r="E21" s="146" t="s">
+      <c r="E21" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="64"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="161" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="92"/>
-      <c r="J21" s="92"/>
-      <c r="K21" s="162"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="96"/>
       <c r="L21" s="43" t="s">
         <v>108</v>
       </c>
       <c r="M21" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="O21" s="49"/>
+      <c r="O21" s="67"/>
     </row>
     <row r="22" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>1.6</v>
       </c>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="64"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="65"/>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="92"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="161" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" s="92"/>
-      <c r="J22" s="92"/>
-      <c r="K22" s="162"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="93"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="96"/>
       <c r="L22" s="43" t="s">
         <v>108</v>
       </c>
       <c r="M22" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="O22" s="49"/>
+      <c r="O22" s="67"/>
     </row>
     <row r="23" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <v>1.7</v>
       </c>
-      <c r="B23" s="143" t="s">
+      <c r="B23" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="140"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="110" t="s">
+      <c r="C23" s="112"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="108"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="163" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="109"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="127" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="128"/>
       <c r="L23" s="44" t="s">
         <v>108</v>
       </c>
       <c r="M23" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="O23" s="49"/>
+      <c r="O23" s="67"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20">
         <v>2</v>
       </c>
-      <c r="B24" s="156" t="s">
+      <c r="B24" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="157"/>
-      <c r="L24" s="157"/>
-      <c r="M24" s="158"/>
-      <c r="O24" s="49"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="109"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="109"/>
+      <c r="M24" s="110"/>
+      <c r="O24" s="67"/>
     </row>
     <row r="25" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22">
         <v>2.1</v>
       </c>
-      <c r="B25" s="151" t="s">
+      <c r="B25" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="152"/>
-      <c r="D25" s="153"/>
-      <c r="E25" s="154" t="s">
+      <c r="C25" s="104"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="155"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="56"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="74"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
-      <c r="O25" s="50"/>
+      <c r="O25" s="68"/>
     </row>
     <row r="26" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B26" s="142" t="s">
+      <c r="B26" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="140"/>
-      <c r="D26" s="141"/>
-      <c r="E26" s="143" t="s">
+      <c r="C26" s="112"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="140"/>
-      <c r="G26" s="141"/>
-      <c r="H26" s="139"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="141"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="133"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="113"/>
       <c r="L26" s="23"/>
       <c r="M26" s="23"/>
       <c r="O26" s="2"/>
@@ -2953,41 +2953,41 @@
       <c r="A27" s="20">
         <v>3</v>
       </c>
-      <c r="B27" s="144" t="s">
+      <c r="B27" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="145"/>
-      <c r="I27" s="145"/>
-      <c r="J27" s="145"/>
-      <c r="K27" s="145"/>
-      <c r="L27" s="145"/>
-      <c r="M27" s="62"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="78"/>
     </row>
     <row r="28" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>3.1</v>
       </c>
-      <c r="B28" s="97" t="s">
+      <c r="B28" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="94" t="s">
+      <c r="C28" s="52"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="95"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="166"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="118"/>
       <c r="L28" s="45" t="s">
         <v>108</v>
       </c>
@@ -2999,22 +2999,22 @@
       <c r="A29" s="15">
         <v>3.2</v>
       </c>
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="64"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="65"/>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="92"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="166"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I29" s="117"/>
+      <c r="J29" s="117"/>
+      <c r="K29" s="118"/>
       <c r="L29" s="45" t="s">
         <v>108</v>
       </c>
@@ -3026,22 +3026,22 @@
       <c r="A30" s="15">
         <v>3.3</v>
       </c>
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="64"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="65"/>
-      <c r="E30" s="91" t="s">
+      <c r="E30" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="92"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="166"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="117"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="118"/>
       <c r="L30" s="45" t="s">
         <v>108</v>
       </c>
@@ -3053,22 +3053,22 @@
       <c r="A31" s="21">
         <v>3.4</v>
       </c>
-      <c r="B31" s="132" t="s">
+      <c r="B31" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="133"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="85" t="s">
+      <c r="C31" s="120"/>
+      <c r="D31" s="121"/>
+      <c r="E31" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="86"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="166"/>
+      <c r="F31" s="122"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="117"/>
+      <c r="J31" s="117"/>
+      <c r="K31" s="118"/>
       <c r="L31" s="45" t="s">
         <v>108</v>
       </c>
@@ -3080,22 +3080,22 @@
       <c r="A32" s="21">
         <v>3.5</v>
       </c>
-      <c r="B32" s="114" t="s">
+      <c r="B32" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="115"/>
-      <c r="D32" s="116"/>
-      <c r="E32" s="114" t="s">
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="115"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="166"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" s="117"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="118"/>
       <c r="L32" s="45" t="s">
         <v>108</v>
       </c>
@@ -3107,41 +3107,41 @@
       <c r="A33" s="25">
         <v>4</v>
       </c>
-      <c r="B33" s="135" t="s">
+      <c r="B33" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="136"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="136"/>
-      <c r="H33" s="136"/>
-      <c r="I33" s="136"/>
-      <c r="J33" s="136"/>
-      <c r="K33" s="136"/>
-      <c r="L33" s="136"/>
-      <c r="M33" s="137"/>
+      <c r="C33" s="164"/>
+      <c r="D33" s="164"/>
+      <c r="E33" s="164"/>
+      <c r="F33" s="164"/>
+      <c r="G33" s="164"/>
+      <c r="H33" s="164"/>
+      <c r="I33" s="164"/>
+      <c r="J33" s="164"/>
+      <c r="K33" s="164"/>
+      <c r="L33" s="164"/>
+      <c r="M33" s="165"/>
     </row>
     <row r="34" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="94" t="s">
+      <c r="C34" s="52"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="95"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="166"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="131"/>
+      <c r="H34" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="118"/>
       <c r="L34" s="45" t="s">
         <v>108</v>
       </c>
@@ -3153,22 +3153,22 @@
       <c r="A35" s="15">
         <v>4.2</v>
       </c>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="64"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="65"/>
-      <c r="E35" s="94" t="s">
+      <c r="E35" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="95"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" s="95"/>
-      <c r="J35" s="95"/>
-      <c r="K35" s="166"/>
+      <c r="F35" s="117"/>
+      <c r="G35" s="131"/>
+      <c r="H35" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="118"/>
       <c r="L35" s="45" t="s">
         <v>108</v>
       </c>
@@ -3180,22 +3180,22 @@
       <c r="A36" s="15">
         <v>4.3</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="64"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="65"/>
-      <c r="E36" s="91" t="s">
+      <c r="E36" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="92"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I36" s="95"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="166"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I36" s="117"/>
+      <c r="J36" s="117"/>
+      <c r="K36" s="118"/>
       <c r="L36" s="45" t="s">
         <v>108</v>
       </c>
@@ -3207,22 +3207,22 @@
       <c r="A37" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="64"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="65"/>
-      <c r="E37" s="91" t="s">
+      <c r="E37" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="92"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I37" s="95"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="166"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" s="117"/>
+      <c r="J37" s="117"/>
+      <c r="K37" s="118"/>
       <c r="L37" s="45" t="s">
         <v>108</v>
       </c>
@@ -3234,22 +3234,22 @@
       <c r="A38" s="21">
         <v>4.5</v>
       </c>
-      <c r="B38" s="132" t="s">
+      <c r="B38" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="133"/>
-      <c r="D38" s="134"/>
-      <c r="E38" s="94" t="s">
+      <c r="C38" s="120"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="95"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I38" s="95"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="166"/>
+      <c r="F38" s="117"/>
+      <c r="G38" s="131"/>
+      <c r="H38" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="117"/>
+      <c r="J38" s="117"/>
+      <c r="K38" s="118"/>
       <c r="L38" s="45" t="s">
         <v>108</v>
       </c>
@@ -3261,22 +3261,22 @@
       <c r="A39" s="21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B39" s="132" t="s">
+      <c r="B39" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="133"/>
-      <c r="D39" s="134"/>
-      <c r="E39" s="91" t="s">
+      <c r="C39" s="120"/>
+      <c r="D39" s="121"/>
+      <c r="E39" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="92"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="166"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="94"/>
+      <c r="H39" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="118"/>
       <c r="L39" s="45" t="s">
         <v>108</v>
       </c>
@@ -3288,22 +3288,22 @@
       <c r="A40" s="21">
         <v>4.7</v>
       </c>
-      <c r="B40" s="88" t="s">
+      <c r="B40" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="64"/>
+      <c r="C40" s="55"/>
       <c r="D40" s="65"/>
-      <c r="E40" s="91" t="s">
+      <c r="E40" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="92"/>
-      <c r="G40" s="93"/>
-      <c r="H40" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I40" s="95"/>
-      <c r="J40" s="95"/>
-      <c r="K40" s="166"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="94"/>
+      <c r="H40" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I40" s="117"/>
+      <c r="J40" s="117"/>
+      <c r="K40" s="118"/>
       <c r="L40" s="45" t="s">
         <v>108</v>
       </c>
@@ -3315,22 +3315,22 @@
       <c r="A41" s="21">
         <v>4.8</v>
       </c>
-      <c r="B41" s="88" t="s">
+      <c r="B41" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="64"/>
+      <c r="C41" s="55"/>
       <c r="D41" s="65"/>
-      <c r="E41" s="91" t="s">
+      <c r="E41" s="92" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="92"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I41" s="95"/>
-      <c r="J41" s="95"/>
-      <c r="K41" s="166"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="94"/>
+      <c r="H41" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="117"/>
+      <c r="J41" s="117"/>
+      <c r="K41" s="118"/>
       <c r="L41" s="45" t="s">
         <v>108</v>
       </c>
@@ -3342,22 +3342,22 @@
       <c r="A42" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B42" s="132" t="s">
+      <c r="B42" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="133"/>
-      <c r="D42" s="134"/>
-      <c r="E42" s="94" t="s">
+      <c r="C42" s="120"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="95"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="166"/>
+      <c r="F42" s="117"/>
+      <c r="G42" s="131"/>
+      <c r="H42" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I42" s="117"/>
+      <c r="J42" s="117"/>
+      <c r="K42" s="118"/>
       <c r="L42" s="45" t="s">
         <v>108</v>
       </c>
@@ -3369,22 +3369,22 @@
       <c r="A43" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B43" s="132" t="s">
+      <c r="B43" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="133"/>
-      <c r="D43" s="134"/>
-      <c r="E43" s="91" t="s">
+      <c r="C43" s="120"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="92"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I43" s="95"/>
-      <c r="J43" s="95"/>
-      <c r="K43" s="166"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I43" s="117"/>
+      <c r="J43" s="117"/>
+      <c r="K43" s="118"/>
       <c r="L43" s="45" t="s">
         <v>108</v>
       </c>
@@ -3396,22 +3396,22 @@
       <c r="A44" s="21">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B44" s="88" t="s">
+      <c r="B44" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="64"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="65"/>
-      <c r="E44" s="91" t="s">
+      <c r="E44" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="92"/>
-      <c r="G44" s="93"/>
-      <c r="H44" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="166"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I44" s="117"/>
+      <c r="J44" s="117"/>
+      <c r="K44" s="118"/>
       <c r="L44" s="45" t="s">
         <v>108</v>
       </c>
@@ -3423,22 +3423,22 @@
       <c r="A45" s="29">
         <v>4.12</v>
       </c>
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="108"/>
-      <c r="D45" s="109"/>
-      <c r="E45" s="110" t="s">
+      <c r="C45" s="125"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="108"/>
-      <c r="G45" s="109"/>
-      <c r="H45" s="165" t="s">
-        <v>108</v>
-      </c>
-      <c r="I45" s="95"/>
-      <c r="J45" s="95"/>
-      <c r="K45" s="166"/>
+      <c r="F45" s="125"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="117"/>
+      <c r="J45" s="117"/>
+      <c r="K45" s="118"/>
       <c r="L45" s="45" t="s">
         <v>108</v>
       </c>
@@ -3450,39 +3450,39 @@
       <c r="A46" s="25">
         <v>5</v>
       </c>
-      <c r="B46" s="117" t="s">
+      <c r="B46" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="118"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118"/>
-      <c r="J46" s="118"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="118"/>
-      <c r="M46" s="119"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="141"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="141"/>
+      <c r="G46" s="141"/>
+      <c r="H46" s="141"/>
+      <c r="I46" s="141"/>
+      <c r="J46" s="141"/>
+      <c r="K46" s="141"/>
+      <c r="L46" s="141"/>
+      <c r="M46" s="142"/>
     </row>
     <row r="47" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B47" s="120" t="s">
+      <c r="B47" s="148" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="121"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="120" t="s">
+      <c r="C47" s="149"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="148" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="121"/>
-      <c r="G47" s="122"/>
-      <c r="H47" s="123"/>
-      <c r="I47" s="123"/>
-      <c r="J47" s="123"/>
-      <c r="K47" s="123"/>
+      <c r="F47" s="149"/>
+      <c r="G47" s="150"/>
+      <c r="H47" s="154"/>
+      <c r="I47" s="154"/>
+      <c r="J47" s="154"/>
+      <c r="K47" s="154"/>
       <c r="L47" s="30"/>
       <c r="M47" s="32" t="s">
         <v>60</v>
@@ -3492,20 +3492,20 @@
       <c r="A48" s="28">
         <v>5.2</v>
       </c>
-      <c r="B48" s="104" t="s">
+      <c r="B48" s="144" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="105"/>
-      <c r="D48" s="106"/>
-      <c r="E48" s="104" t="s">
+      <c r="C48" s="145"/>
+      <c r="D48" s="146"/>
+      <c r="E48" s="144" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="105"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="124"/>
-      <c r="I48" s="124"/>
-      <c r="J48" s="124"/>
-      <c r="K48" s="124"/>
+      <c r="F48" s="145"/>
+      <c r="G48" s="146"/>
+      <c r="H48" s="143"/>
+      <c r="I48" s="143"/>
+      <c r="J48" s="143"/>
+      <c r="K48" s="143"/>
       <c r="L48" s="19"/>
       <c r="M48" s="16"/>
     </row>
@@ -3513,20 +3513,20 @@
       <c r="A49" s="28">
         <v>5.3</v>
       </c>
-      <c r="B49" s="104" t="s">
+      <c r="B49" s="144" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="105"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="104" t="s">
+      <c r="C49" s="145"/>
+      <c r="D49" s="146"/>
+      <c r="E49" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="105"/>
-      <c r="G49" s="106"/>
-      <c r="H49" s="124"/>
-      <c r="I49" s="124"/>
-      <c r="J49" s="124"/>
-      <c r="K49" s="124"/>
+      <c r="F49" s="145"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="143"/>
+      <c r="I49" s="143"/>
+      <c r="J49" s="143"/>
+      <c r="K49" s="143"/>
       <c r="L49" s="19"/>
       <c r="M49" s="16"/>
     </row>
@@ -3534,20 +3534,20 @@
       <c r="A50" s="29">
         <v>5.4</v>
       </c>
-      <c r="B50" s="114" t="s">
+      <c r="B50" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="115"/>
-      <c r="D50" s="116"/>
-      <c r="E50" s="114" t="s">
+      <c r="C50" s="114"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="F50" s="115"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
-      <c r="K50" s="113"/>
+      <c r="F50" s="114"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="151"/>
+      <c r="I50" s="152"/>
+      <c r="J50" s="152"/>
+      <c r="K50" s="153"/>
       <c r="L50" s="23"/>
       <c r="M50" s="16"/>
     </row>
@@ -3555,39 +3555,39 @@
       <c r="A51" s="25">
         <v>6</v>
       </c>
-      <c r="B51" s="117" t="s">
+      <c r="B51" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="118"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
-      <c r="I51" s="118"/>
-      <c r="J51" s="118"/>
-      <c r="K51" s="118"/>
-      <c r="L51" s="118"/>
-      <c r="M51" s="119"/>
+      <c r="C51" s="141"/>
+      <c r="D51" s="141"/>
+      <c r="E51" s="141"/>
+      <c r="F51" s="141"/>
+      <c r="G51" s="141"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
+      <c r="J51" s="141"/>
+      <c r="K51" s="141"/>
+      <c r="L51" s="141"/>
+      <c r="M51" s="142"/>
     </row>
     <row r="52" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
         <v>6.1</v>
       </c>
-      <c r="B52" s="80" t="s">
+      <c r="B52" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="81"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="80" t="s">
+      <c r="C52" s="161"/>
+      <c r="D52" s="162"/>
+      <c r="E52" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="F52" s="81"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="101"/>
-      <c r="I52" s="102"/>
-      <c r="J52" s="102"/>
-      <c r="K52" s="103"/>
+      <c r="F52" s="161"/>
+      <c r="G52" s="162"/>
+      <c r="H52" s="158"/>
+      <c r="I52" s="159"/>
+      <c r="J52" s="159"/>
+      <c r="K52" s="160"/>
       <c r="L52" s="30"/>
       <c r="M52" s="33"/>
     </row>
@@ -3595,20 +3595,20 @@
       <c r="A53" s="28">
         <v>6.2</v>
       </c>
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="86"/>
-      <c r="D53" s="87"/>
-      <c r="E53" s="85" t="s">
+      <c r="C53" s="122"/>
+      <c r="D53" s="123"/>
+      <c r="E53" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="F53" s="86"/>
-      <c r="G53" s="87"/>
-      <c r="H53" s="98"/>
-      <c r="I53" s="99"/>
-      <c r="J53" s="99"/>
-      <c r="K53" s="100"/>
+      <c r="F53" s="122"/>
+      <c r="G53" s="123"/>
+      <c r="H53" s="155"/>
+      <c r="I53" s="156"/>
+      <c r="J53" s="156"/>
+      <c r="K53" s="157"/>
       <c r="L53" s="19"/>
       <c r="M53" s="16"/>
     </row>
@@ -3616,20 +3616,20 @@
       <c r="A54" s="28">
         <v>6.3</v>
       </c>
-      <c r="B54" s="80" t="s">
+      <c r="B54" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="81"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="80" t="s">
+      <c r="C54" s="161"/>
+      <c r="D54" s="162"/>
+      <c r="E54" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="F54" s="81"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="98"/>
-      <c r="I54" s="99"/>
-      <c r="J54" s="99"/>
-      <c r="K54" s="100"/>
+      <c r="F54" s="161"/>
+      <c r="G54" s="162"/>
+      <c r="H54" s="155"/>
+      <c r="I54" s="156"/>
+      <c r="J54" s="156"/>
+      <c r="K54" s="157"/>
       <c r="L54" s="19"/>
       <c r="M54" s="16"/>
     </row>
@@ -3637,35 +3637,35 @@
       <c r="A55" s="28">
         <v>6.4</v>
       </c>
-      <c r="B55" s="104" t="s">
+      <c r="B55" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="105"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="104" t="s">
+      <c r="C55" s="145"/>
+      <c r="D55" s="146"/>
+      <c r="E55" s="144" t="s">
         <v>76</v>
       </c>
-      <c r="F55" s="105"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="124"/>
-      <c r="I55" s="124"/>
-      <c r="J55" s="124"/>
-      <c r="K55" s="124"/>
+      <c r="F55" s="145"/>
+      <c r="G55" s="146"/>
+      <c r="H55" s="143"/>
+      <c r="I55" s="143"/>
+      <c r="J55" s="143"/>
+      <c r="K55" s="143"/>
       <c r="L55" s="19"/>
       <c r="M55" s="16"/>
     </row>
     <row r="56" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
-      <c r="B56" s="125"/>
-      <c r="C56" s="126"/>
-      <c r="D56" s="127"/>
-      <c r="E56" s="128"/>
-      <c r="F56" s="126"/>
-      <c r="G56" s="127"/>
-      <c r="H56" s="129"/>
-      <c r="I56" s="130"/>
-      <c r="J56" s="130"/>
-      <c r="K56" s="131"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="135"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="135"/>
+      <c r="G56" s="136"/>
+      <c r="H56" s="138"/>
+      <c r="I56" s="139"/>
+      <c r="J56" s="139"/>
+      <c r="K56" s="140"/>
       <c r="L56" s="17"/>
       <c r="M56" s="6"/>
     </row>
@@ -3697,31 +3697,108 @@
     </row>
   </sheetData>
   <mergeCells count="151">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="B27:M27"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="H20:K20"/>
@@ -3746,108 +3823,31 @@
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:K22"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="B51:M51"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>